<commit_message>
more detailed mobile cases
</commit_message>
<xml_diff>
--- a/cases_mobile.xlsx
+++ b/cases_mobile.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="57">
   <si>
     <t>Test Scenario ID</t>
   </si>
@@ -189,6 +189,12 @@
   </si>
   <si>
     <t>Don't fill the inputs and click signup button</t>
+  </si>
+  <si>
+    <t>Profile Page</t>
+  </si>
+  <si>
+    <t>Click profile navigation button</t>
   </si>
 </sst>
 </file>
@@ -633,7 +639,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -778,6 +784,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1060,10 +1078,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I52"/>
+  <dimension ref="B1:I57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1198,46 +1216,46 @@
       </c>
     </row>
     <row r="8" spans="2:9" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>2</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="53" t="s">
         <v>20</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="47" t="s">
-        <v>24</v>
+        <v>55</v>
+      </c>
+      <c r="F8" s="55" t="s">
+        <v>55</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="H8" s="50" t="s">
+      <c r="H8" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="24" t="s">
+      <c r="I8" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:9" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>21</v>
+        <v>39</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>20</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F9" s="47" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>52</v>
@@ -1249,81 +1267,89 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="3">
+    <row r="10" spans="2:9" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="2">
         <v>3</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="H10" s="50" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" ht="46.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="3">
+        <v>3</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D11" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="48" t="s">
+      <c r="F11" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G11" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="H10" s="51" t="s">
+      <c r="H11" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="I10" s="21" t="s">
+      <c r="I11" s="21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="2:9" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="25" t="s">
+    <row r="12" spans="2:9" ht="32.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C13" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="27" t="s">
+      <c r="D13" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="28" t="s">
+      <c r="E13" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="38"/>
-    </row>
-    <row r="13" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="29" t="s">
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="38"/>
+    </row>
+    <row r="14" spans="2:9" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C14" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="31" t="s">
+      <c r="D14" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="32" t="s">
+      <c r="E14" s="32" t="s">
         <v>6</v>
-      </c>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="40"/>
-    </row>
-    <row r="14" spans="2:9" ht="41.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="36" t="s">
-        <v>8</v>
       </c>
       <c r="F14" s="39"/>
       <c r="G14" s="39"/>
@@ -1331,653 +1357,779 @@
       <c r="I14" s="40"/>
     </row>
     <row r="15" spans="2:9" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="43" t="s">
+      <c r="B15" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="40"/>
+    </row>
+    <row r="16" spans="2:9" ht="22.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="44"/>
-      <c r="D15" s="44"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="42"/>
-    </row>
-    <row r="16" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="11" t="s">
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="42"/>
+    </row>
+    <row r="17" spans="2:9" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C17" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D17" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E17" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="F17" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="G17" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H16" s="12" t="s">
+      <c r="H17" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="I16" s="11" t="s">
+      <c r="I17" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="2:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="1">
+    <row r="18" spans="2:9" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="1">
         <v>1</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C18" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="D18" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="E17" s="18" t="s">
+      <c r="E18" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="F17" s="18" t="s">
+      <c r="F18" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="G17" s="20" t="s">
+      <c r="G18" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="H17" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B18" s="2">
-        <v>2</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="H18" s="9" t="s">
+      <c r="H18" s="8" t="s">
         <v>18</v>
       </c>
       <c r="I18" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="2:9" ht="133.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="3">
+    <row r="19" spans="2:9" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="1">
+        <v>2</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="53" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" s="55" t="s">
+        <v>55</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B20" s="2">
         <v>3</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C20" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" ht="127.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="3">
+        <v>4</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D21" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E21" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F21" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G19" s="7" t="s">
+      <c r="G21" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="H19" s="10" t="s">
+      <c r="H21" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="I19" s="7" t="s">
+      <c r="I21" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="24" spans="2:9" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="25" t="s">
+    <row r="24" spans="2:9" ht="19.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="2:9" ht="19.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="2:9" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C24" s="26" t="s">
+      <c r="C26" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="27" t="s">
+      <c r="D26" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="28" t="s">
+      <c r="E26" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="F24" s="37"/>
-      <c r="G24" s="37"/>
-      <c r="H24" s="37"/>
-      <c r="I24" s="38"/>
-    </row>
-    <row r="25" spans="2:9" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="29" t="s">
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="38"/>
+    </row>
+    <row r="27" spans="2:9" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="30" t="s">
+      <c r="C27" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="D25" s="31" t="s">
+      <c r="D27" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="E25" s="32" t="s">
+      <c r="E27" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="F25" s="39"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="39"/>
-      <c r="I25" s="40"/>
-    </row>
-    <row r="26" spans="2:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="33" t="s">
+      <c r="F27" s="39"/>
+      <c r="G27" s="39"/>
+      <c r="H27" s="39"/>
+      <c r="I27" s="40"/>
+    </row>
+    <row r="28" spans="2:9" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="34" t="s">
+      <c r="C28" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="D26" s="35" t="s">
+      <c r="D28" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="E26" s="36" t="s">
+      <c r="E28" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="F26" s="39"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="39"/>
-      <c r="I26" s="40"/>
-    </row>
-    <row r="27" spans="2:9" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="43" t="s">
+      <c r="F28" s="39"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="39"/>
+      <c r="I28" s="40"/>
+    </row>
+    <row r="29" spans="2:9" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="44"/>
-      <c r="D27" s="44"/>
-      <c r="E27" s="45"/>
-      <c r="F27" s="41"/>
-      <c r="G27" s="41"/>
-      <c r="H27" s="41"/>
-      <c r="I27" s="42"/>
-    </row>
-    <row r="28" spans="2:9" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="11" t="s">
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="41"/>
+      <c r="G29" s="41"/>
+      <c r="H29" s="41"/>
+      <c r="I29" s="42"/>
+    </row>
+    <row r="30" spans="2:9" ht="41.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C30" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D28" s="11" t="s">
+      <c r="D30" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E28" s="11" t="s">
+      <c r="E30" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F28" s="11" t="s">
+      <c r="F30" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G28" s="11" t="s">
+      <c r="G30" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H28" s="12" t="s">
+      <c r="H30" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="I28" s="11" t="s">
+      <c r="I30" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="2:9" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="1">
+    <row r="31" spans="2:9" ht="85.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="1">
         <v>1</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C31" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="D29" s="19" t="s">
+      <c r="D31" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="E29" s="18" t="s">
+      <c r="E31" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="F29" s="18" t="s">
+      <c r="F31" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="G29" s="20" t="s">
+      <c r="G31" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="H29" s="8" t="s">
+      <c r="H31" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="I29" s="6" t="s">
+      <c r="I31" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="2:9" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="2">
+    <row r="32" spans="2:9" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="1">
         <v>2</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C32" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D32" s="53" t="s">
+        <v>20</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F32" s="55" t="s">
+        <v>55</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="H32" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="2">
+        <v>3</v>
+      </c>
+      <c r="C33" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D30" s="15" t="s">
+      <c r="D33" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E30" s="13" t="s">
+      <c r="E33" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="F30" s="14" t="s">
+      <c r="F33" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G30" s="6" t="s">
+      <c r="G33" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="H30" s="9" t="s">
+      <c r="H33" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I30" s="6" t="s">
+      <c r="I33" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="2:9" ht="85.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="3">
+    <row r="34" spans="2:9" ht="94.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B34" s="3">
+        <v>4</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H34" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I34" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" ht="61.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="2:9" ht="41.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="37" spans="2:9" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="D37" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="F37" s="37"/>
+      <c r="G37" s="37"/>
+      <c r="H37" s="37"/>
+      <c r="I37" s="38"/>
+    </row>
+    <row r="38" spans="2:9" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D38" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="F38" s="39"/>
+      <c r="G38" s="39"/>
+      <c r="H38" s="39"/>
+      <c r="I38" s="40"/>
+    </row>
+    <row r="39" spans="2:9" ht="49.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B39" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="F39" s="39"/>
+      <c r="G39" s="39"/>
+      <c r="H39" s="39"/>
+      <c r="I39" s="40"/>
+    </row>
+    <row r="40" spans="2:9" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B40" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" s="44"/>
+      <c r="D40" s="44"/>
+      <c r="E40" s="45"/>
+      <c r="F40" s="41"/>
+      <c r="G40" s="41"/>
+      <c r="H40" s="41"/>
+      <c r="I40" s="42"/>
+    </row>
+    <row r="41" spans="2:9" ht="85.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B41" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H41" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="I41" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="1">
+        <v>1</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D42" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="E42" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="F42" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="G42" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="H42" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I42" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="1">
+        <v>2</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D43" s="53" t="s">
+        <v>20</v>
+      </c>
+      <c r="E43" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F43" s="55" t="s">
+        <v>55</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="H43" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I43" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="2">
         <v>3</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G31" s="7" t="s">
+      <c r="C44" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D44" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E44" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F44" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G44" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="H31" s="10" t="s">
+      <c r="H44" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I31" s="7" t="s">
+      <c r="I44" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="34" spans="2:9" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="25" t="s">
+    <row r="45" spans="2:9" ht="90.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B45" s="3">
+        <v>4</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H45" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I45" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="2:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="2:9" ht="22.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="49" spans="2:9" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C34" s="26" t="s">
+      <c r="C49" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="D34" s="27" t="s">
+      <c r="D49" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="E34" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="F34" s="37"/>
-      <c r="G34" s="37"/>
-      <c r="H34" s="37"/>
-      <c r="I34" s="38"/>
-    </row>
-    <row r="35" spans="2:9" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="29" t="s">
+      <c r="E49" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F49" s="37"/>
+      <c r="G49" s="37"/>
+      <c r="H49" s="37"/>
+      <c r="I49" s="38"/>
+    </row>
+    <row r="50" spans="2:9" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C35" s="30" t="s">
+      <c r="C50" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="D35" s="31" t="s">
+      <c r="D50" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="E35" s="32" t="s">
+      <c r="E50" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="F35" s="39"/>
-      <c r="G35" s="39"/>
-      <c r="H35" s="39"/>
-      <c r="I35" s="40"/>
-    </row>
-    <row r="36" spans="2:9" ht="41.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="33" t="s">
+      <c r="F50" s="39"/>
+      <c r="G50" s="39"/>
+      <c r="H50" s="39"/>
+      <c r="I50" s="40"/>
+    </row>
+    <row r="51" spans="2:9" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B51" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="C36" s="34" t="s">
+      <c r="C51" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="D36" s="35" t="s">
+      <c r="D51" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="E36" s="36" t="s">
+      <c r="E51" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="F36" s="39"/>
-      <c r="G36" s="39"/>
-      <c r="H36" s="39"/>
-      <c r="I36" s="40"/>
-    </row>
-    <row r="37" spans="2:9" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="43" t="s">
+      <c r="F51" s="39"/>
+      <c r="G51" s="39"/>
+      <c r="H51" s="39"/>
+      <c r="I51" s="40"/>
+    </row>
+    <row r="52" spans="2:9" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B52" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="C37" s="44"/>
-      <c r="D37" s="44"/>
-      <c r="E37" s="45"/>
-      <c r="F37" s="41"/>
-      <c r="G37" s="41"/>
-      <c r="H37" s="41"/>
-      <c r="I37" s="42"/>
-    </row>
-    <row r="38" spans="2:9" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="11" t="s">
+      <c r="C52" s="44"/>
+      <c r="D52" s="44"/>
+      <c r="E52" s="45"/>
+      <c r="F52" s="41"/>
+      <c r="G52" s="41"/>
+      <c r="H52" s="41"/>
+      <c r="I52" s="42"/>
+    </row>
+    <row r="53" spans="2:9" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B53" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="C53" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D38" s="11" t="s">
+      <c r="D53" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E38" s="11" t="s">
+      <c r="E53" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F38" s="11" t="s">
+      <c r="F53" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G38" s="11" t="s">
+      <c r="G53" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="H38" s="12" t="s">
+      <c r="H53" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="I38" s="11" t="s">
+      <c r="I53" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="2:9" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="1">
+    <row r="54" spans="2:9" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="1">
         <v>1</v>
       </c>
-      <c r="C39" s="13" t="s">
+      <c r="C54" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="D39" s="19" t="s">
+      <c r="D54" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="E39" s="18" t="s">
+      <c r="E54" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="F39" s="18" t="s">
+      <c r="F54" s="54" t="s">
         <v>53</v>
       </c>
-      <c r="G39" s="20" t="s">
+      <c r="G54" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="H39" s="8" t="s">
+      <c r="H54" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="I39" s="6" t="s">
+      <c r="I54" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="2:9" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="2">
+    <row r="55" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B55" s="1">
         <v>2</v>
       </c>
-      <c r="C40" s="13" t="s">
+      <c r="C55" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D55" s="53" t="s">
+        <v>20</v>
+      </c>
+      <c r="E55" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F55" s="55" t="s">
+        <v>55</v>
+      </c>
+      <c r="G55" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="H55" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I55" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="56" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B56" s="2">
+        <v>3</v>
+      </c>
+      <c r="C56" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D40" s="15" t="s">
+      <c r="D56" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E40" s="13" t="s">
+      <c r="E56" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="F40" s="14" t="s">
+      <c r="F56" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="G40" s="6" t="s">
+      <c r="G56" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="H40" s="9" t="s">
+      <c r="H56" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I40" s="6" t="s">
+      <c r="I56" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="2:9" ht="85.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="3">
-        <v>3</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G41" s="7" t="s">
+    <row r="57" spans="2:9" ht="101.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B57" s="3">
+        <v>4</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F57" s="56" t="s">
+        <v>48</v>
+      </c>
+      <c r="G57" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="H41" s="10" t="s">
+      <c r="H57" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="I41" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="44" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="45" spans="2:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C45" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="D45" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="E45" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="F45" s="37"/>
-      <c r="G45" s="37"/>
-      <c r="H45" s="37"/>
-      <c r="I45" s="38"/>
-    </row>
-    <row r="46" spans="2:9" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="C46" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="D46" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="E46" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="F46" s="39"/>
-      <c r="G46" s="39"/>
-      <c r="H46" s="39"/>
-      <c r="I46" s="40"/>
-    </row>
-    <row r="47" spans="2:9" ht="28.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="C47" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="D47" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="E47" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="F47" s="39"/>
-      <c r="G47" s="39"/>
-      <c r="H47" s="39"/>
-      <c r="I47" s="40"/>
-    </row>
-    <row r="48" spans="2:9" ht="22.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B48" s="43" t="s">
-        <v>9</v>
-      </c>
-      <c r="C48" s="44"/>
-      <c r="D48" s="44"/>
-      <c r="E48" s="45"/>
-      <c r="F48" s="41"/>
-      <c r="G48" s="41"/>
-      <c r="H48" s="41"/>
-      <c r="I48" s="42"/>
-    </row>
-    <row r="49" spans="2:9" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B49" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C49" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D49" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E49" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F49" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="G49" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="H49" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="I49" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="50" spans="2:9" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="1">
-        <v>1</v>
-      </c>
-      <c r="C50" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="D50" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="E50" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="F50" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="G50" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="H50" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="I50" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="51" spans="2:9" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="2">
-        <v>2</v>
-      </c>
-      <c r="C51" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D51" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E51" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="F51" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="G51" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="H51" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I51" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="52" spans="2:9" ht="81" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B52" s="3">
-        <v>3</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E52" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F52" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="G52" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="H52" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="I52" s="7" t="s">
+      <c r="I57" s="7" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="F34:I37"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="F45:I48"/>
-    <mergeCell ref="B48:E48"/>
+    <mergeCell ref="F37:I40"/>
+    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="F49:I52"/>
+    <mergeCell ref="B52:E52"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="F2:I5"/>
-    <mergeCell ref="F12:I15"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="F24:I27"/>
-    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="F13:I16"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="F26:I29"/>
+    <mergeCell ref="B29:E29"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D7" r:id="rId1" display="https://m.apkpure.com/tr/lc-waikiki/com.lcwaikiki.android"/>
-    <hyperlink ref="D17" r:id="rId2" display="https://m.apkpure.com/tr/lc-waikiki/com.lcwaikiki.android"/>
-    <hyperlink ref="D29" r:id="rId3" display="https://m.apkpure.com/tr/lc-waikiki/com.lcwaikiki.android"/>
-    <hyperlink ref="D39" r:id="rId4" display="https://m.apkpure.com/tr/lc-waikiki/com.lcwaikiki.android"/>
-    <hyperlink ref="D50" r:id="rId5" display="https://m.apkpure.com/tr/lc-waikiki/com.lcwaikiki.android"/>
+    <hyperlink ref="D18" r:id="rId2" display="https://m.apkpure.com/tr/lc-waikiki/com.lcwaikiki.android"/>
+    <hyperlink ref="D31" r:id="rId3" display="https://m.apkpure.com/tr/lc-waikiki/com.lcwaikiki.android"/>
+    <hyperlink ref="D42" r:id="rId4" display="https://m.apkpure.com/tr/lc-waikiki/com.lcwaikiki.android"/>
+    <hyperlink ref="D54" r:id="rId5" display="https://m.apkpure.com/tr/lc-waikiki/com.lcwaikiki.android"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>

</xml_diff>